<commit_message>
UPDATED GBDS ZIP 04-03-2025
</commit_message>
<xml_diff>
--- a/PROMO ISSUANCE AND RECEIPTS MONITORING.xlsx
+++ b/PROMO ISSUANCE AND RECEIPTS MONITORING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703809DF-B704-4B89-9280-7DB63A31A581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2143A349-F799-4953-898D-1B6C055BBCB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{90A4BF69-F41C-4D57-82A3-8979CB5194E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="132">
   <si>
     <t>GUILLERMO BEVERAGE DISTRIBUTION SERVICES</t>
   </si>
@@ -328,6 +328,108 @@
   </si>
   <si>
     <t>10 BOTTLES</t>
+  </si>
+  <si>
+    <t>03/14/2025</t>
+  </si>
+  <si>
+    <t>03/15/2025</t>
+  </si>
+  <si>
+    <t>RSHL</t>
+  </si>
+  <si>
+    <t>03/17/2025</t>
+  </si>
+  <si>
+    <t>03/18/2025</t>
+  </si>
+  <si>
+    <t>03/19/2025</t>
+  </si>
+  <si>
+    <t>PP1000</t>
+  </si>
+  <si>
+    <t>03/20/2025</t>
+  </si>
+  <si>
+    <t>03/26/2025</t>
+  </si>
+  <si>
+    <t>03/29/2025</t>
+  </si>
+  <si>
+    <t>03/21/2025</t>
+  </si>
+  <si>
+    <t>03/22/2025</t>
+  </si>
+  <si>
+    <t>RHS330</t>
+  </si>
+  <si>
+    <t>03/24/2025</t>
+  </si>
+  <si>
+    <t>03/25/2025</t>
+  </si>
+  <si>
+    <t>03/27/2025</t>
+  </si>
+  <si>
+    <t>03/28/2025</t>
+  </si>
+  <si>
+    <t>03/31/2025</t>
+  </si>
+  <si>
+    <t>outlet name</t>
+  </si>
+  <si>
+    <t>barangay</t>
+  </si>
+  <si>
+    <t>promo title</t>
+  </si>
+  <si>
+    <t>bro store</t>
+  </si>
+  <si>
+    <t>sindangan</t>
+  </si>
+  <si>
+    <t>janyna store</t>
+  </si>
+  <si>
+    <t>taboada</t>
+  </si>
+  <si>
+    <t>lbp</t>
+  </si>
+  <si>
+    <t>ambus store</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>invoice no.</t>
+  </si>
+  <si>
+    <t>TATA &amp; ELLY</t>
+  </si>
+  <si>
+    <t>SALUG</t>
+  </si>
+  <si>
+    <t>0000328</t>
+  </si>
+  <si>
+    <t>jn &amp; son store</t>
+  </si>
+  <si>
+    <t>0000605</t>
   </si>
 </sst>
 </file>
@@ -338,7 +440,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +483,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -414,7 +523,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -539,12 +648,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -639,6 +792,45 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,9 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -969,13 +1158,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38022B2-4D09-4C9B-A1E8-728962E58E2E}">
-  <dimension ref="A1:O123"/>
+  <dimension ref="A1:R185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H117" sqref="H117"/>
+      <selection pane="bottomRight" activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -991,95 +1180,115 @@
     <col min="10" max="10" width="8.5703125" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="12">
-        <f>SUM(C7:C191)</f>
-        <v>163258</v>
+        <f>SUM(C7:C212)</f>
+        <v>229045</v>
       </c>
       <c r="D4" s="12">
-        <f>SUM(D7:D191)</f>
-        <v>135888</v>
+        <f>SUM(D7:D212)</f>
+        <v>154963</v>
       </c>
       <c r="E4" s="13">
         <f>D4-C4</f>
-        <v>-27370</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+        <v>-74082</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="47"/>
+      <c r="E5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="45" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="32"/>
+      <c r="O5" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="R5" s="45" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45391</v>
       </c>
@@ -1104,7 +1313,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45421</v>
       </c>
@@ -1129,7 +1338,7 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45452</v>
       </c>
@@ -1150,7 +1359,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45452</v>
       </c>
@@ -1175,7 +1384,7 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45635</v>
       </c>
@@ -1200,7 +1409,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1225,7 +1434,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1246,7 +1455,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1275,7 +1484,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1296,7 +1505,7 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -3657,7 +3866,7 @@
       <c r="N109" s="6"/>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A110" s="25">
+      <c r="A110" s="31">
         <v>45719</v>
       </c>
       <c r="B110" s="9" t="s">
@@ -3867,7 +4076,7 @@
       <c r="G117" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H117" s="36" t="s">
+      <c r="H117" s="32" t="s">
         <v>97</v>
       </c>
       <c r="I117" s="6"/>
@@ -3878,13 +4087,23 @@
       <c r="N117" s="6"/>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A118" s="25"/>
-      <c r="B118" s="9"/>
-      <c r="C118" s="11"/>
+      <c r="A118" s="25">
+        <v>45994</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C118" s="11">
+        <v>325</v>
+      </c>
       <c r="D118" s="11"/>
       <c r="E118" s="6"/>
-      <c r="G118" s="6"/>
-      <c r="H118" s="6"/>
+      <c r="G118" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H118" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="I118" s="6"/>
       <c r="J118" s="6"/>
       <c r="K118" s="6"/>
@@ -3893,13 +4112,23 @@
       <c r="N118" s="6"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A119" s="25"/>
-      <c r="B119" s="9"/>
-      <c r="C119" s="11"/>
+      <c r="A119" s="25">
+        <v>45994</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C119" s="11">
+        <v>500</v>
+      </c>
       <c r="D119" s="11"/>
       <c r="E119" s="6"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="6"/>
+      <c r="G119" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H119" s="6">
+        <v>1</v>
+      </c>
       <c r="I119" s="6"/>
       <c r="J119" s="6"/>
       <c r="K119" s="6"/>
@@ -3908,28 +4137,52 @@
       <c r="N119" s="6"/>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A120" s="25"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="11"/>
+      <c r="A120" s="25">
+        <v>45994</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C120" s="11">
+        <v>825</v>
+      </c>
       <c r="D120" s="11"/>
       <c r="E120" s="6"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
-      <c r="I120" s="6"/>
-      <c r="J120" s="6"/>
+      <c r="G120" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H120" s="6">
+        <v>1</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J120" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="K120" s="6"/>
       <c r="L120" s="6"/>
       <c r="M120" s="6"/>
       <c r="N120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A121" s="25"/>
-      <c r="B121" s="9"/>
-      <c r="C121" s="11"/>
+      <c r="A121" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C121" s="11">
+        <v>674</v>
+      </c>
       <c r="D121" s="11"/>
       <c r="E121" s="6"/>
-      <c r="G121" s="6"/>
-      <c r="H121" s="6"/>
+      <c r="G121" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H121" s="6">
+        <v>1</v>
+      </c>
       <c r="I121" s="6"/>
       <c r="J121" s="6"/>
       <c r="K121" s="6"/>
@@ -3938,13 +4191,23 @@
       <c r="N121" s="6"/>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A122" s="25"/>
-      <c r="B122" s="9"/>
-      <c r="C122" s="11"/>
+      <c r="A122" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C122" s="11">
+        <v>674</v>
+      </c>
       <c r="D122" s="11"/>
       <c r="E122" s="6"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
+      <c r="G122" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H122" s="6">
+        <v>1</v>
+      </c>
       <c r="I122" s="6"/>
       <c r="J122" s="6"/>
       <c r="K122" s="6"/>
@@ -3953,13 +4216,23 @@
       <c r="N122" s="6"/>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A123" s="25"/>
-      <c r="B123" s="9"/>
-      <c r="C123" s="11"/>
+      <c r="A123" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C123" s="11">
+        <v>500</v>
+      </c>
       <c r="D123" s="11"/>
       <c r="E123" s="6"/>
-      <c r="G123" s="6"/>
-      <c r="H123" s="6"/>
+      <c r="G123" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H123" s="6">
+        <v>1</v>
+      </c>
       <c r="I123" s="6"/>
       <c r="J123" s="6"/>
       <c r="K123" s="6"/>
@@ -3967,14 +4240,1551 @@
       <c r="M123" s="6"/>
       <c r="N123" s="6"/>
     </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A124" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B124" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C124" s="11">
+        <v>674</v>
+      </c>
+      <c r="D124" s="11"/>
+      <c r="E124" s="6"/>
+      <c r="G124" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H124" s="6">
+        <v>1</v>
+      </c>
+      <c r="I124" s="6"/>
+      <c r="J124" s="6"/>
+      <c r="K124" s="6"/>
+      <c r="L124" s="6"/>
+      <c r="M124" s="6"/>
+      <c r="N124" s="6"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A125" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C125" s="11">
+        <v>825</v>
+      </c>
+      <c r="D125" s="11"/>
+      <c r="E125" s="6"/>
+      <c r="G125" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H125" s="6">
+        <v>1</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J125" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K125" s="6"/>
+      <c r="L125" s="6"/>
+      <c r="M125" s="6"/>
+      <c r="N125" s="6"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A126" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C126" s="11">
+        <v>500</v>
+      </c>
+      <c r="D126" s="11"/>
+      <c r="E126" s="6"/>
+      <c r="G126" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H126" s="6">
+        <v>1</v>
+      </c>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
+      <c r="N126" s="6"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A127" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C127" s="11">
+        <v>1096</v>
+      </c>
+      <c r="D127" s="11"/>
+      <c r="E127" s="6"/>
+      <c r="G127" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H127" s="6">
+        <v>1</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J127" s="6">
+        <v>1</v>
+      </c>
+      <c r="K127" s="6"/>
+      <c r="L127" s="6"/>
+      <c r="M127" s="6"/>
+      <c r="N127" s="6"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A128" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C128" s="11">
+        <v>325</v>
+      </c>
+      <c r="D128" s="11"/>
+      <c r="E128" s="6"/>
+      <c r="G128" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H128" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I128" s="6"/>
+      <c r="J128" s="6"/>
+      <c r="K128" s="6"/>
+      <c r="L128" s="6"/>
+      <c r="M128" s="6"/>
+      <c r="N128" s="6"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A129" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="11">
+        <f>559*20</f>
+        <v>11180</v>
+      </c>
+      <c r="D129" s="11"/>
+      <c r="E129" s="6"/>
+      <c r="G129" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H129" s="6">
+        <v>20</v>
+      </c>
+      <c r="I129" s="6"/>
+      <c r="J129" s="6"/>
+      <c r="K129" s="6"/>
+      <c r="L129" s="6"/>
+      <c r="M129" s="6"/>
+      <c r="N129" s="6"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A130" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C130" s="11">
+        <v>674</v>
+      </c>
+      <c r="D130" s="11"/>
+      <c r="E130" s="6"/>
+      <c r="G130" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H130" s="6">
+        <v>1</v>
+      </c>
+      <c r="I130" s="6"/>
+      <c r="J130" s="6"/>
+      <c r="K130" s="6"/>
+      <c r="L130" s="6"/>
+      <c r="M130" s="6"/>
+      <c r="N130" s="6"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A131" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C131" s="11">
+        <v>674</v>
+      </c>
+      <c r="D131" s="11"/>
+      <c r="E131" s="6"/>
+      <c r="G131" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H131" s="6">
+        <v>1</v>
+      </c>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+      <c r="K131" s="6"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
+      <c r="N131" s="6"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A132" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B132" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C132" s="11">
+        <v>674</v>
+      </c>
+      <c r="D132" s="11"/>
+      <c r="E132" s="6"/>
+      <c r="G132" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H132" s="6">
+        <v>1</v>
+      </c>
+      <c r="I132" s="6"/>
+      <c r="J132" s="6"/>
+      <c r="K132" s="6"/>
+      <c r="L132" s="6"/>
+      <c r="M132" s="6"/>
+      <c r="N132" s="6"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A133" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C133" s="11">
+        <f>15*913</f>
+        <v>13695</v>
+      </c>
+      <c r="D133" s="11"/>
+      <c r="E133" s="6"/>
+      <c r="G133" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H133" s="6">
+        <v>15</v>
+      </c>
+      <c r="I133" s="6"/>
+      <c r="J133" s="6"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+      <c r="N133" s="6"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A134" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C134" s="11">
+        <v>674</v>
+      </c>
+      <c r="D134" s="11"/>
+      <c r="E134" s="6"/>
+      <c r="G134" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H134" s="6">
+        <v>1</v>
+      </c>
+      <c r="I134" s="6"/>
+      <c r="J134" s="6"/>
+      <c r="K134" s="6"/>
+      <c r="L134" s="6"/>
+      <c r="M134" s="6"/>
+      <c r="N134" s="6"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A135" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C135" s="11">
+        <v>674</v>
+      </c>
+      <c r="D135" s="11"/>
+      <c r="E135" s="6"/>
+      <c r="G135" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H135" s="6">
+        <v>1</v>
+      </c>
+      <c r="I135" s="6"/>
+      <c r="J135" s="6"/>
+      <c r="K135" s="6"/>
+      <c r="L135" s="6"/>
+      <c r="M135" s="6"/>
+      <c r="N135" s="6"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A136" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C136" s="11">
+        <f>596+325</f>
+        <v>921</v>
+      </c>
+      <c r="D136" s="11"/>
+      <c r="E136" s="6"/>
+      <c r="G136" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H136" s="6">
+        <v>1</v>
+      </c>
+      <c r="I136" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J136" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K136" s="6"/>
+      <c r="L136" s="6"/>
+      <c r="M136" s="6"/>
+      <c r="N136" s="6"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A137" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C137" s="11">
+        <f>913*4</f>
+        <v>3652</v>
+      </c>
+      <c r="D137" s="11"/>
+      <c r="E137" s="6"/>
+      <c r="G137" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H137" s="6">
+        <v>4</v>
+      </c>
+      <c r="I137" s="6"/>
+      <c r="J137" s="6"/>
+      <c r="K137" s="6"/>
+      <c r="L137" s="6"/>
+      <c r="M137" s="6"/>
+      <c r="N137" s="6"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A138" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C138" s="11">
+        <f>674+596+626</f>
+        <v>1896</v>
+      </c>
+      <c r="D138" s="11"/>
+      <c r="E138" s="6"/>
+      <c r="G138" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H138" s="6">
+        <v>1</v>
+      </c>
+      <c r="I138" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J138" s="6">
+        <v>1</v>
+      </c>
+      <c r="K138" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L138" s="6">
+        <v>1</v>
+      </c>
+      <c r="M138" s="6"/>
+      <c r="N138" s="6"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A139" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C139" s="11">
+        <f>596+674</f>
+        <v>1270</v>
+      </c>
+      <c r="D139" s="11"/>
+      <c r="E139" s="6"/>
+      <c r="G139" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H139" s="6">
+        <v>1</v>
+      </c>
+      <c r="I139" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J139" s="6">
+        <v>1</v>
+      </c>
+      <c r="K139" s="6"/>
+      <c r="L139" s="6"/>
+      <c r="M139" s="6"/>
+      <c r="N139" s="6"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A140" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C140" s="11">
+        <f>674+325</f>
+        <v>999</v>
+      </c>
+      <c r="D140" s="11"/>
+      <c r="E140" s="6"/>
+      <c r="G140" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H140" s="6">
+        <v>1</v>
+      </c>
+      <c r="I140" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J140" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K140" s="6"/>
+      <c r="L140" s="6"/>
+      <c r="M140" s="6"/>
+      <c r="N140" s="6"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A141" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B141" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11">
+        <v>3250</v>
+      </c>
+      <c r="E141" s="6"/>
+      <c r="G141" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H141" s="16">
+        <v>5</v>
+      </c>
+      <c r="I141" s="6"/>
+      <c r="J141" s="30"/>
+      <c r="K141" s="6"/>
+      <c r="L141" s="6"/>
+      <c r="M141" s="6"/>
+      <c r="N141" s="6"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A142" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B142" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11">
+        <v>4825</v>
+      </c>
+      <c r="E142" s="6"/>
+      <c r="G142" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H142" s="16">
+        <v>2</v>
+      </c>
+      <c r="I142" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J142" s="33">
+        <v>3</v>
+      </c>
+      <c r="K142" s="6"/>
+      <c r="L142" s="6"/>
+      <c r="M142" s="6"/>
+      <c r="N142" s="6"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A143" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B143" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11">
+        <v>11000</v>
+      </c>
+      <c r="E143" s="6"/>
+      <c r="G143" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H143" s="16">
+        <v>22</v>
+      </c>
+      <c r="I143" s="6"/>
+      <c r="J143" s="30"/>
+      <c r="K143" s="6"/>
+      <c r="L143" s="6"/>
+      <c r="M143" s="6"/>
+      <c r="N143" s="6"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A144" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C144" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D144" s="11"/>
+      <c r="E144" s="6"/>
+      <c r="G144" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H144" s="6">
+        <v>2</v>
+      </c>
+      <c r="I144" s="6"/>
+      <c r="J144" s="6"/>
+      <c r="K144" s="6"/>
+      <c r="L144" s="6"/>
+      <c r="M144" s="6"/>
+      <c r="N144" s="6"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C145" s="11">
+        <f>596</f>
+        <v>596</v>
+      </c>
+      <c r="D145" s="11"/>
+      <c r="E145" s="6"/>
+      <c r="G145" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H145" s="6">
+        <v>1</v>
+      </c>
+      <c r="I145" s="6"/>
+      <c r="J145" s="6"/>
+      <c r="K145" s="6"/>
+      <c r="L145" s="6"/>
+      <c r="M145" s="6"/>
+      <c r="N145" s="6"/>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A146" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C146" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D146" s="11"/>
+      <c r="E146" s="6"/>
+      <c r="G146" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H146" s="6">
+        <v>2</v>
+      </c>
+      <c r="I146" s="6"/>
+      <c r="J146" s="6"/>
+      <c r="K146" s="6"/>
+      <c r="L146" s="6"/>
+      <c r="M146" s="6"/>
+      <c r="N146" s="6"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C147" s="11">
+        <v>1252</v>
+      </c>
+      <c r="D147" s="11"/>
+      <c r="E147" s="6"/>
+      <c r="G147" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H147" s="6">
+        <v>2</v>
+      </c>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="6"/>
+      <c r="M147" s="6"/>
+      <c r="N147" s="6"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A148" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C148" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D148" s="11"/>
+      <c r="E148" s="6"/>
+      <c r="G148" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H148" s="6">
+        <v>2</v>
+      </c>
+      <c r="I148" s="6"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="6"/>
+      <c r="L148" s="6"/>
+      <c r="M148" s="6"/>
+      <c r="N148" s="6"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A149" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C149" s="11">
+        <f>626*2+674*2</f>
+        <v>2600</v>
+      </c>
+      <c r="D149" s="11"/>
+      <c r="E149" s="6"/>
+      <c r="G149" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H149" s="6">
+        <v>2</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J149" s="6">
+        <v>2</v>
+      </c>
+      <c r="K149" s="6"/>
+      <c r="L149" s="6"/>
+      <c r="M149" s="6"/>
+      <c r="N149" s="6"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A150" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C150" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D150" s="11"/>
+      <c r="E150" s="6"/>
+      <c r="G150" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H150" s="6">
+        <v>2</v>
+      </c>
+      <c r="I150" s="6"/>
+      <c r="J150" s="6"/>
+      <c r="K150" s="6"/>
+      <c r="L150" s="6"/>
+      <c r="M150" s="6"/>
+      <c r="N150" s="6"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A151" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C151" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D151" s="11"/>
+      <c r="E151" s="6"/>
+      <c r="G151" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H151" s="6">
+        <v>2</v>
+      </c>
+      <c r="I151" s="6"/>
+      <c r="J151" s="6"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="6"/>
+      <c r="M151" s="6"/>
+      <c r="N151" s="6"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A152" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B152" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C152" s="37">
+        <f>626*2+626*2+674*2+626</f>
+        <v>4478</v>
+      </c>
+      <c r="D152" s="36"/>
+      <c r="E152" s="38"/>
+      <c r="G152" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="H152" s="38">
+        <v>5</v>
+      </c>
+      <c r="I152" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="J152" s="38">
+        <v>2</v>
+      </c>
+      <c r="K152" s="38"/>
+      <c r="L152" s="38"/>
+      <c r="M152" s="38"/>
+      <c r="N152" s="38"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A153" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B153" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C153" s="34">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D153" s="11"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
+      <c r="G153" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H153" s="6">
+        <v>2</v>
+      </c>
+      <c r="I153" s="6"/>
+      <c r="J153" s="6"/>
+      <c r="K153" s="6"/>
+      <c r="L153" s="6"/>
+      <c r="M153" s="6"/>
+      <c r="N153" s="6"/>
+      <c r="O153" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P153" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q153" s="6"/>
+      <c r="R153" s="44"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B154" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C154" s="34">
+        <f>674*2</f>
+        <v>1348</v>
+      </c>
+      <c r="D154" s="11"/>
+      <c r="E154" s="6"/>
+      <c r="F154" s="6"/>
+      <c r="G154" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H154" s="6">
+        <v>2</v>
+      </c>
+      <c r="I154" s="6"/>
+      <c r="J154" s="6"/>
+      <c r="K154" s="6"/>
+      <c r="L154" s="6"/>
+      <c r="M154" s="6"/>
+      <c r="N154" s="6"/>
+      <c r="O154" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P154" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q154" s="6"/>
+      <c r="R154" s="44"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B155" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="C155" s="34">
+        <v>500</v>
+      </c>
+      <c r="D155" s="11"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="6"/>
+      <c r="G155" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H155" s="6">
+        <v>1</v>
+      </c>
+      <c r="I155" s="6"/>
+      <c r="J155" s="6"/>
+      <c r="K155" s="6"/>
+      <c r="L155" s="6"/>
+      <c r="M155" s="6"/>
+      <c r="N155" s="6"/>
+      <c r="O155" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P155" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q155" s="6"/>
+      <c r="R155" s="44"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C156" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D156" s="11"/>
+      <c r="E156" s="6"/>
+      <c r="F156" s="6"/>
+      <c r="G156" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H156" s="43">
+        <v>2</v>
+      </c>
+      <c r="I156" s="6"/>
+      <c r="J156" s="6"/>
+      <c r="K156" s="6"/>
+      <c r="L156" s="6"/>
+      <c r="M156" s="6"/>
+      <c r="N156" s="6"/>
+      <c r="O156" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="P156" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q156" s="6"/>
+      <c r="R156" s="44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C157" s="11">
+        <f>596</f>
+        <v>596</v>
+      </c>
+      <c r="D157" s="11"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="6"/>
+      <c r="G157" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H157" s="6">
+        <v>1</v>
+      </c>
+      <c r="I157" s="6"/>
+      <c r="J157" s="6"/>
+      <c r="K157" s="6"/>
+      <c r="L157" s="6"/>
+      <c r="M157" s="6"/>
+      <c r="N157" s="6"/>
+      <c r="O157" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="P157" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q157" s="6"/>
+      <c r="R157" s="44"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C158" s="11">
+        <f>500</f>
+        <v>500</v>
+      </c>
+      <c r="D158" s="11"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H158" s="6">
+        <v>1</v>
+      </c>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6"/>
+      <c r="K158" s="6"/>
+      <c r="L158" s="6"/>
+      <c r="M158" s="6"/>
+      <c r="N158" s="6"/>
+      <c r="O158" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="P158" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q158" s="6"/>
+      <c r="R158" s="44"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C159" s="11">
+        <f>626*2</f>
+        <v>1252</v>
+      </c>
+      <c r="D159" s="11"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H159" s="6">
+        <v>2</v>
+      </c>
+      <c r="I159" s="6"/>
+      <c r="J159" s="6"/>
+      <c r="K159" s="6"/>
+      <c r="L159" s="6"/>
+      <c r="M159" s="6"/>
+      <c r="N159" s="6"/>
+      <c r="O159" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P159" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q159" s="6"/>
+      <c r="R159" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A160" s="2"/>
+      <c r="B160" s="11"/>
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="6"/>
+      <c r="J160" s="6"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="6"/>
+      <c r="M160" s="6"/>
+      <c r="N160" s="6"/>
+      <c r="O160" s="6"/>
+      <c r="P160" s="6"/>
+      <c r="Q160" s="6"/>
+      <c r="R160" s="6"/>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A161" s="2"/>
+      <c r="B161" s="11"/>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11"/>
+      <c r="E161" s="6"/>
+      <c r="F161" s="6"/>
+      <c r="G161" s="6"/>
+      <c r="H161" s="6"/>
+      <c r="I161" s="6"/>
+      <c r="J161" s="6"/>
+      <c r="K161" s="6"/>
+      <c r="L161" s="6"/>
+      <c r="M161" s="6"/>
+      <c r="N161" s="6"/>
+      <c r="O161" s="6"/>
+      <c r="P161" s="6"/>
+      <c r="Q161" s="6"/>
+      <c r="R161" s="6"/>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A162" s="2"/>
+      <c r="B162" s="11"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="6"/>
+      <c r="F162" s="6"/>
+      <c r="G162" s="6"/>
+      <c r="H162" s="6"/>
+      <c r="I162" s="6"/>
+      <c r="J162" s="6"/>
+      <c r="K162" s="6"/>
+      <c r="L162" s="6"/>
+      <c r="M162" s="6"/>
+      <c r="N162" s="6"/>
+      <c r="O162" s="6"/>
+      <c r="P162" s="6"/>
+      <c r="Q162" s="6"/>
+      <c r="R162" s="6"/>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+      <c r="B163" s="11"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="6"/>
+      <c r="F163" s="6"/>
+      <c r="G163" s="6"/>
+      <c r="H163" s="6"/>
+      <c r="I163" s="6"/>
+      <c r="J163" s="6"/>
+      <c r="K163" s="6"/>
+      <c r="L163" s="6"/>
+      <c r="M163" s="6"/>
+      <c r="N163" s="6"/>
+      <c r="O163" s="6"/>
+      <c r="P163" s="6"/>
+      <c r="Q163" s="6"/>
+      <c r="R163" s="6"/>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A164" s="2"/>
+      <c r="B164" s="11"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11"/>
+      <c r="E164" s="6"/>
+      <c r="F164" s="6"/>
+      <c r="G164" s="6"/>
+      <c r="H164" s="6"/>
+      <c r="I164" s="6"/>
+      <c r="J164" s="6"/>
+      <c r="K164" s="6"/>
+      <c r="L164" s="6"/>
+      <c r="M164" s="6"/>
+      <c r="N164" s="6"/>
+      <c r="O164" s="6"/>
+      <c r="P164" s="6"/>
+      <c r="Q164" s="6"/>
+      <c r="R164" s="6"/>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A165" s="2"/>
+      <c r="B165" s="11"/>
+      <c r="C165" s="11"/>
+      <c r="D165" s="11"/>
+      <c r="E165" s="6"/>
+      <c r="F165" s="6"/>
+      <c r="G165" s="6"/>
+      <c r="H165" s="6"/>
+      <c r="I165" s="6"/>
+      <c r="J165" s="6"/>
+      <c r="K165" s="6"/>
+      <c r="L165" s="6"/>
+      <c r="M165" s="6"/>
+      <c r="N165" s="6"/>
+      <c r="O165" s="6"/>
+      <c r="P165" s="6"/>
+      <c r="Q165" s="6"/>
+      <c r="R165" s="6"/>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A166" s="2"/>
+      <c r="B166" s="11"/>
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="6"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="6"/>
+      <c r="H166" s="6"/>
+      <c r="I166" s="6"/>
+      <c r="J166" s="6"/>
+      <c r="K166" s="6"/>
+      <c r="L166" s="6"/>
+      <c r="M166" s="6"/>
+      <c r="N166" s="6"/>
+      <c r="O166" s="6"/>
+      <c r="P166" s="6"/>
+      <c r="Q166" s="6"/>
+      <c r="R166" s="6"/>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A167" s="2"/>
+      <c r="B167" s="11"/>
+      <c r="C167" s="11"/>
+      <c r="D167" s="11"/>
+      <c r="E167" s="6"/>
+      <c r="F167" s="6"/>
+      <c r="G167" s="6"/>
+      <c r="H167" s="6"/>
+      <c r="I167" s="6"/>
+      <c r="J167" s="6"/>
+      <c r="K167" s="6"/>
+      <c r="L167" s="6"/>
+      <c r="M167" s="6"/>
+      <c r="N167" s="6"/>
+      <c r="O167" s="6"/>
+      <c r="P167" s="6"/>
+      <c r="Q167" s="6"/>
+      <c r="R167" s="6"/>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A168" s="2"/>
+      <c r="B168" s="11"/>
+      <c r="C168" s="11"/>
+      <c r="D168" s="11"/>
+      <c r="E168" s="6"/>
+      <c r="F168" s="6"/>
+      <c r="G168" s="6"/>
+      <c r="H168" s="6"/>
+      <c r="I168" s="6"/>
+      <c r="J168" s="6"/>
+      <c r="K168" s="6"/>
+      <c r="L168" s="6"/>
+      <c r="M168" s="6"/>
+      <c r="N168" s="6"/>
+      <c r="O168" s="6"/>
+      <c r="P168" s="6"/>
+      <c r="Q168" s="6"/>
+      <c r="R168" s="6"/>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A169" s="2"/>
+      <c r="B169" s="11"/>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
+      <c r="G169" s="6"/>
+      <c r="H169" s="6"/>
+      <c r="I169" s="6"/>
+      <c r="J169" s="6"/>
+      <c r="K169" s="6"/>
+      <c r="L169" s="6"/>
+      <c r="M169" s="6"/>
+      <c r="N169" s="6"/>
+      <c r="O169" s="6"/>
+      <c r="P169" s="6"/>
+      <c r="Q169" s="6"/>
+      <c r="R169" s="6"/>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A170" s="2"/>
+      <c r="B170" s="11"/>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="6"/>
+      <c r="J170" s="6"/>
+      <c r="K170" s="6"/>
+      <c r="L170" s="6"/>
+      <c r="M170" s="6"/>
+      <c r="N170" s="6"/>
+      <c r="O170" s="6"/>
+      <c r="P170" s="6"/>
+      <c r="Q170" s="6"/>
+      <c r="R170" s="6"/>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A171" s="2"/>
+      <c r="B171" s="11"/>
+      <c r="C171" s="11"/>
+      <c r="D171" s="11"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="6"/>
+      <c r="I171" s="6"/>
+      <c r="J171" s="6"/>
+      <c r="K171" s="6"/>
+      <c r="L171" s="6"/>
+      <c r="M171" s="6"/>
+      <c r="N171" s="6"/>
+      <c r="O171" s="6"/>
+      <c r="P171" s="6"/>
+      <c r="Q171" s="6"/>
+      <c r="R171" s="6"/>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A172" s="2"/>
+      <c r="B172" s="11"/>
+      <c r="C172" s="11"/>
+      <c r="D172" s="11"/>
+      <c r="E172" s="6"/>
+      <c r="F172" s="6"/>
+      <c r="G172" s="6"/>
+      <c r="H172" s="6"/>
+      <c r="I172" s="6"/>
+      <c r="J172" s="6"/>
+      <c r="K172" s="6"/>
+      <c r="L172" s="6"/>
+      <c r="M172" s="6"/>
+      <c r="N172" s="6"/>
+      <c r="O172" s="6"/>
+      <c r="P172" s="6"/>
+      <c r="Q172" s="6"/>
+      <c r="R172" s="6"/>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A173" s="2"/>
+      <c r="B173" s="11"/>
+      <c r="C173" s="11"/>
+      <c r="D173" s="11"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+      <c r="J173" s="6"/>
+      <c r="K173" s="6"/>
+      <c r="L173" s="6"/>
+      <c r="M173" s="6"/>
+      <c r="N173" s="6"/>
+      <c r="O173" s="6"/>
+      <c r="P173" s="6"/>
+      <c r="Q173" s="6"/>
+      <c r="R173" s="6"/>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+      <c r="B174" s="11"/>
+      <c r="C174" s="11"/>
+      <c r="D174" s="11"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+      <c r="J174" s="6"/>
+      <c r="K174" s="6"/>
+      <c r="L174" s="6"/>
+      <c r="M174" s="6"/>
+      <c r="N174" s="6"/>
+      <c r="O174" s="6"/>
+      <c r="P174" s="6"/>
+      <c r="Q174" s="6"/>
+      <c r="R174" s="6"/>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A175" s="2"/>
+      <c r="B175" s="11"/>
+      <c r="C175" s="11"/>
+      <c r="D175" s="11"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="6"/>
+      <c r="H175" s="6"/>
+      <c r="I175" s="6"/>
+      <c r="J175" s="6"/>
+      <c r="K175" s="6"/>
+      <c r="L175" s="6"/>
+      <c r="M175" s="6"/>
+      <c r="N175" s="6"/>
+      <c r="O175" s="6"/>
+      <c r="P175" s="6"/>
+      <c r="Q175" s="6"/>
+      <c r="R175" s="6"/>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A176" s="2"/>
+      <c r="B176" s="11"/>
+      <c r="C176" s="11"/>
+      <c r="D176" s="11"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
+      <c r="G176" s="6"/>
+      <c r="H176" s="6"/>
+      <c r="I176" s="6"/>
+      <c r="J176" s="6"/>
+      <c r="K176" s="6"/>
+      <c r="L176" s="6"/>
+      <c r="M176" s="6"/>
+      <c r="N176" s="6"/>
+      <c r="O176" s="6"/>
+      <c r="P176" s="6"/>
+      <c r="Q176" s="6"/>
+      <c r="R176" s="6"/>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A177" s="2"/>
+      <c r="B177" s="11"/>
+      <c r="C177" s="11"/>
+      <c r="D177" s="11"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
+      <c r="G177" s="6"/>
+      <c r="H177" s="6"/>
+      <c r="I177" s="6"/>
+      <c r="J177" s="6"/>
+      <c r="K177" s="6"/>
+      <c r="L177" s="6"/>
+      <c r="M177" s="6"/>
+      <c r="N177" s="6"/>
+      <c r="O177" s="6"/>
+      <c r="P177" s="6"/>
+      <c r="Q177" s="6"/>
+      <c r="R177" s="6"/>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A178" s="39"/>
+      <c r="B178" s="40"/>
+      <c r="C178" s="41"/>
+      <c r="D178" s="41"/>
+      <c r="E178" s="42"/>
+      <c r="G178" s="42"/>
+      <c r="H178" s="42"/>
+      <c r="I178" s="42"/>
+      <c r="J178" s="42"/>
+      <c r="K178" s="42"/>
+      <c r="L178" s="42"/>
+      <c r="M178" s="42"/>
+      <c r="N178" s="42"/>
+      <c r="O178" s="6"/>
+      <c r="P178" s="6"/>
+      <c r="Q178" s="6"/>
+      <c r="R178" s="6"/>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A179" s="25"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="11"/>
+      <c r="D179" s="11"/>
+      <c r="E179" s="6"/>
+      <c r="G179" s="6"/>
+      <c r="H179" s="6"/>
+      <c r="I179" s="6"/>
+      <c r="J179" s="6"/>
+      <c r="K179" s="6"/>
+      <c r="L179" s="6"/>
+      <c r="M179" s="6"/>
+      <c r="N179" s="6"/>
+      <c r="O179" s="6"/>
+      <c r="P179" s="6"/>
+      <c r="Q179" s="6"/>
+      <c r="R179" s="6"/>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A180" s="25"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="11"/>
+      <c r="D180" s="11"/>
+      <c r="E180" s="6"/>
+      <c r="G180" s="6"/>
+      <c r="H180" s="6"/>
+      <c r="I180" s="6"/>
+      <c r="J180" s="6"/>
+      <c r="K180" s="6"/>
+      <c r="L180" s="6"/>
+      <c r="M180" s="6"/>
+      <c r="N180" s="6"/>
+      <c r="O180" s="6"/>
+      <c r="P180" s="6"/>
+      <c r="Q180" s="6"/>
+      <c r="R180" s="6"/>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A181" s="25"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11"/>
+      <c r="E181" s="6"/>
+      <c r="G181" s="6"/>
+      <c r="H181" s="6"/>
+      <c r="I181" s="6"/>
+      <c r="J181" s="6"/>
+      <c r="K181" s="6"/>
+      <c r="L181" s="6"/>
+      <c r="M181" s="6"/>
+      <c r="N181" s="6"/>
+      <c r="O181" s="6"/>
+      <c r="P181" s="6"/>
+      <c r="Q181" s="6"/>
+      <c r="R181" s="6"/>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A182" s="25"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="11"/>
+      <c r="D182" s="11"/>
+      <c r="E182" s="6"/>
+      <c r="G182" s="6"/>
+      <c r="H182" s="6"/>
+      <c r="I182" s="6"/>
+      <c r="J182" s="6"/>
+      <c r="K182" s="6"/>
+      <c r="L182" s="6"/>
+      <c r="M182" s="6"/>
+      <c r="N182" s="6"/>
+      <c r="O182" s="6"/>
+      <c r="P182" s="6"/>
+      <c r="Q182" s="6"/>
+      <c r="R182" s="6"/>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A183" s="25"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
+      <c r="E183" s="6"/>
+      <c r="G183" s="6"/>
+      <c r="H183" s="6"/>
+      <c r="I183" s="6"/>
+      <c r="J183" s="6"/>
+      <c r="K183" s="6"/>
+      <c r="L183" s="6"/>
+      <c r="M183" s="6"/>
+      <c r="N183" s="6"/>
+      <c r="O183" s="6"/>
+      <c r="P183" s="6"/>
+      <c r="Q183" s="6"/>
+      <c r="R183" s="6"/>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A184" s="25"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
+      <c r="E184" s="6"/>
+      <c r="G184" s="6"/>
+      <c r="H184" s="6"/>
+      <c r="I184" s="6"/>
+      <c r="J184" s="6"/>
+      <c r="K184" s="6"/>
+      <c r="L184" s="6"/>
+      <c r="M184" s="6"/>
+      <c r="N184" s="6"/>
+      <c r="O184" s="6"/>
+      <c r="P184" s="6"/>
+      <c r="Q184" s="6"/>
+      <c r="R184" s="6"/>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A185" s="25"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="11"/>
+      <c r="D185" s="11"/>
+      <c r="E185" s="6"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="6"/>
+      <c r="I185" s="6"/>
+      <c r="J185" s="6"/>
+      <c r="K185" s="6"/>
+      <c r="L185" s="6"/>
+      <c r="M185" s="6"/>
+      <c r="N185" s="6"/>
+      <c r="O185" s="6"/>
+      <c r="P185" s="6"/>
+      <c r="Q185" s="6"/>
+      <c r="R185" s="6"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A50:N51">
     <sortCondition ref="B50"/>
   </sortState>
-  <mergeCells count="12">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="G5:G6"/>
+  <mergeCells count="16">
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="N5:N6"/>
@@ -3984,6 +5794,13 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>